<commit_message>
[Jimmy] modificar el excel de carga de creditos_preaprobados_empleados_v.xlsx
</commit_message>
<xml_diff>
--- a/src/assets/anexos/creditos_preaprobados_empleados_v.xlsx
+++ b/src/assets/anexos/creditos_preaprobados_empleados_v.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/papamactwo/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/papamacone/Documents/Edgar/grp-front-center/src/assets/anexos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAE310C8-9DBD-A64B-8C11-58966C738843}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8C4F9A3-267B-4C48-8D19-C3AD7CB6E628}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="19880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="19320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Clientes" sheetId="1" r:id="rId1"/>
@@ -133,6 +133,7 @@
         <sz val="11"/>
         <color indexed="11"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>jsyar@pucesi.edu.ec</t>
     </r>
@@ -168,12 +169,14 @@
       <sz val="11"/>
       <color indexed="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
       <color theme="10"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -218,28 +221,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+  <cellXfs count="12">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1406,23 +1408,28 @@
   <dimension ref="A1:V3"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="14.5" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="7" width="10.83203125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="15.6640625" style="1" customWidth="1"/>
-    <col min="9" max="19" width="17.1640625" style="1" customWidth="1"/>
-    <col min="20" max="20" width="27.83203125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" style="9" customWidth="1"/>
+    <col min="2" max="7" width="10.83203125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="15.6640625" style="10" customWidth="1"/>
+    <col min="9" max="11" width="17.1640625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="17.1640625" style="9" customWidth="1"/>
+    <col min="13" max="16" width="17.1640625" style="1" customWidth="1"/>
+    <col min="17" max="18" width="17.1640625" style="10" customWidth="1"/>
+    <col min="19" max="19" width="17.1640625" style="1" customWidth="1"/>
+    <col min="20" max="20" width="27.83203125" style="10" customWidth="1"/>
     <col min="21" max="21" width="31.6640625" style="1" customWidth="1"/>
-    <col min="22" max="22" width="29.6640625" style="1" customWidth="1"/>
+    <col min="22" max="22" width="29.6640625" style="10" customWidth="1"/>
     <col min="23" max="23" width="10.83203125" style="1" customWidth="1"/>
     <col min="24" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -1455,7 +1462,7 @@
       <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="3" t="s">
         <v>11</v>
       </c>
       <c r="M1" s="2" t="s">
@@ -1514,41 +1521,41 @@
       <c r="H2" s="5">
         <v>1003150602</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="I2" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="J2" s="6" t="s">
+      <c r="J2" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="K2" s="6" t="s">
+      <c r="K2" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="L2" s="7">
+      <c r="L2" s="11">
         <v>36161</v>
       </c>
-      <c r="M2" s="6" t="s">
+      <c r="M2" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="N2" s="6" t="s">
+      <c r="N2" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="O2" s="6" t="s">
+      <c r="O2" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="P2" s="10" t="s">
+      <c r="P2" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="Q2" s="6" t="s">
+      <c r="Q2" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="R2" s="6" t="s">
+      <c r="R2" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="S2" s="9"/>
+      <c r="S2" s="7"/>
       <c r="T2" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="U2" s="6" t="s">
+      <c r="U2" s="5" t="s">
         <v>32</v>
       </c>
       <c r="V2" s="2" t="s">
@@ -1580,41 +1587,41 @@
       <c r="H3" s="5">
         <v>1003150603</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="I3" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="J3" s="6" t="s">
+      <c r="J3" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="K3" s="6" t="s">
+      <c r="K3" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="L3" s="7">
-        <v>36161</v>
-      </c>
-      <c r="M3" s="6" t="s">
+      <c r="L3" s="11">
+        <v>44674</v>
+      </c>
+      <c r="M3" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="N3" s="6" t="s">
+      <c r="N3" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="O3" s="6" t="s">
+      <c r="O3" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="P3" s="8" t="s">
+      <c r="P3" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="Q3" s="6" t="s">
+      <c r="Q3" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="R3" s="6" t="s">
+      <c r="R3" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="S3" s="9"/>
+      <c r="S3" s="7"/>
       <c r="T3" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="U3" s="6" t="s">
+      <c r="U3" s="5" t="s">
         <v>32</v>
       </c>
       <c r="V3" s="2" t="s">

</xml_diff>